<commit_message>
trial 6 - perfect?
</commit_message>
<xml_diff>
--- a/Pearsons_CC/Python_Code/histogram.sample.xlsx
+++ b/Pearsons_CC/Python_Code/histogram.sample.xlsx
@@ -14,15 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Total Iterations</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
 </sst>
 </file>
@@ -239,46 +233,46 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>154</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>10</c:v>
@@ -317,46 +311,46 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>55</c:v>
-                </c:pt>
                 <c:pt idx="38">
-                  <c:v>83</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>92</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>88</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -770,11 +764,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
+      <c r="A1">
+        <v>-1</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -782,7 +776,7 @@
         <v>-0.95</v>
       </c>
       <c r="B2">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -790,7 +784,7 @@
         <v>-0.9</v>
       </c>
       <c r="B3">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -798,7 +792,7 @@
         <v>-0.85</v>
       </c>
       <c r="B4">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -806,7 +800,7 @@
         <v>-0.8</v>
       </c>
       <c r="B5">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -822,7 +816,7 @@
         <v>-0.7</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -830,7 +824,7 @@
         <v>-0.6499999999999999</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -838,7 +832,7 @@
         <v>-0.6</v>
       </c>
       <c r="B9">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -846,7 +840,7 @@
         <v>-0.55</v>
       </c>
       <c r="B10">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -854,7 +848,7 @@
         <v>-0.5</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -862,7 +856,7 @@
         <v>-0.45</v>
       </c>
       <c r="B12">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -870,7 +864,7 @@
         <v>-0.3999999999999999</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -878,7 +872,7 @@
         <v>-0.35</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -886,7 +880,7 @@
         <v>-0.2999999999999999</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -990,7 +984,7 @@
         <v>0.3500000000000001</v>
       </c>
       <c r="B28">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -998,7 +992,7 @@
         <v>0.4000000000000001</v>
       </c>
       <c r="B29">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1006,7 +1000,7 @@
         <v>0.4500000000000002</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1014,7 +1008,7 @@
         <v>0.5</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1022,7 +1016,7 @@
         <v>0.55</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1030,7 +1024,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="B33">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1046,7 +1040,7 @@
         <v>0.7000000000000002</v>
       </c>
       <c r="B35">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1054,7 +1048,7 @@
         <v>0.75</v>
       </c>
       <c r="B36">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1062,7 +1056,7 @@
         <v>0.8</v>
       </c>
       <c r="B37">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1070,7 +1064,7 @@
         <v>0.8500000000000001</v>
       </c>
       <c r="B38">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1078,7 +1072,7 @@
         <v>0.9000000000000001</v>
       </c>
       <c r="B39">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1086,7 +1080,7 @@
         <v>0.9500000000000002</v>
       </c>
       <c r="B40">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1094,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="B41">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:2">

</xml_diff>

<commit_message>
added # of adj. gene airs
</commit_message>
<xml_diff>
--- a/Pearsons_CC/Python_Code/histogram.sample.xlsx
+++ b/Pearsons_CC/Python_Code/histogram.sample.xlsx
@@ -236,124 +236,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>824</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>1413</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>576</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>204</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>219</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>155</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>294</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>206</c:v>
+                  <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>176</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>84</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>196</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>296</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>539</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>543</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>660</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>961</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1439</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1474</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1076</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>725</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>589</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>603</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>522</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>374</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>205</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>85</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>26</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>21</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>51</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>151</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>423</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>874</c:v>
+                  <c:v>412</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2161</c:v>
+                  <c:v>586</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4657</c:v>
+                  <c:v>1146</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9228</c:v>
+                  <c:v>1399</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>70261</c:v>
+                  <c:v>1605</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -779,7 +779,7 @@
         <v>-0.95</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>824</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -787,7 +787,7 @@
         <v>-0.9</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -795,7 +795,7 @@
         <v>-0.85</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -803,7 +803,7 @@
         <v>-0.8</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -811,7 +811,7 @@
         <v>-0.75</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -819,7 +819,7 @@
         <v>-0.7</v>
       </c>
       <c r="B7">
-        <v>70</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -827,7 +827,7 @@
         <v>-0.6499999999999999</v>
       </c>
       <c r="B8">
-        <v>204</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -835,7 +835,7 @@
         <v>-0.6</v>
       </c>
       <c r="B9">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -843,7 +843,7 @@
         <v>-0.55</v>
       </c>
       <c r="B10">
-        <v>155</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -851,7 +851,7 @@
         <v>-0.5</v>
       </c>
       <c r="B11">
-        <v>294</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -859,7 +859,7 @@
         <v>-0.45</v>
       </c>
       <c r="B12">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -867,7 +867,7 @@
         <v>-0.3999999999999999</v>
       </c>
       <c r="B13">
-        <v>176</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -875,7 +875,7 @@
         <v>-0.35</v>
       </c>
       <c r="B14">
-        <v>73</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -883,7 +883,7 @@
         <v>-0.2999999999999999</v>
       </c>
       <c r="B15">
-        <v>84</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -891,7 +891,7 @@
         <v>-0.25</v>
       </c>
       <c r="B16">
-        <v>196</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -899,7 +899,7 @@
         <v>-0.2</v>
       </c>
       <c r="B17">
-        <v>296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -907,7 +907,7 @@
         <v>-0.1499999999999999</v>
       </c>
       <c r="B18">
-        <v>539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -915,7 +915,7 @@
         <v>-0.09999999999999998</v>
       </c>
       <c r="B19">
-        <v>543</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -923,7 +923,7 @@
         <v>-0.04999999999999993</v>
       </c>
       <c r="B20">
-        <v>660</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <v>961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -939,7 +939,7 @@
         <v>0.05000000000000004</v>
       </c>
       <c r="B22">
-        <v>1439</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -947,7 +947,7 @@
         <v>0.1000000000000001</v>
       </c>
       <c r="B23">
-        <v>1474</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -955,7 +955,7 @@
         <v>0.1500000000000001</v>
       </c>
       <c r="B24">
-        <v>1076</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -963,7 +963,7 @@
         <v>0.2000000000000002</v>
       </c>
       <c r="B25">
-        <v>725</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -971,7 +971,7 @@
         <v>0.25</v>
       </c>
       <c r="B26">
-        <v>589</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -979,7 +979,7 @@
         <v>0.3</v>
       </c>
       <c r="B27">
-        <v>603</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -987,7 +987,7 @@
         <v>0.3500000000000001</v>
       </c>
       <c r="B28">
-        <v>522</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -995,7 +995,7 @@
         <v>0.4000000000000001</v>
       </c>
       <c r="B29">
-        <v>374</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1003,7 +1003,7 @@
         <v>0.4500000000000002</v>
       </c>
       <c r="B30">
-        <v>205</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1011,7 +1011,7 @@
         <v>0.5</v>
       </c>
       <c r="B31">
-        <v>85</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1019,7 +1019,7 @@
         <v>0.55</v>
       </c>
       <c r="B32">
-        <v>26</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1027,7 +1027,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1035,7 +1035,7 @@
         <v>0.6500000000000001</v>
       </c>
       <c r="B34">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1043,7 +1043,7 @@
         <v>0.7000000000000002</v>
       </c>
       <c r="B35">
-        <v>151</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1051,7 +1051,7 @@
         <v>0.75</v>
       </c>
       <c r="B36">
-        <v>423</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1059,7 +1059,7 @@
         <v>0.8</v>
       </c>
       <c r="B37">
-        <v>874</v>
+        <v>412</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1067,7 +1067,7 @@
         <v>0.8500000000000001</v>
       </c>
       <c r="B38">
-        <v>2161</v>
+        <v>586</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1075,7 +1075,7 @@
         <v>0.9000000000000001</v>
       </c>
       <c r="B39">
-        <v>4657</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1083,7 +1083,7 @@
         <v>0.9500000000000002</v>
       </c>
       <c r="B40">
-        <v>9228</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1091,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="B41">
-        <v>70261</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="42" spans="1:2">

</xml_diff>

<commit_message>
numbers don't add up
</commit_message>
<xml_diff>
--- a/Pearsons_CC/Python_Code/histogram.sample.xlsx
+++ b/Pearsons_CC/Python_Code/histogram.sample.xlsx
@@ -242,118 +242,118 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>719</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>808</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1080</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>817</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>680</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>353</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>696</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1148</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>2042</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2192</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>2637</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>3872</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>5790</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>6045</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>4763</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>3008</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2</c:v>
+                  <c:v>2435</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>2280</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1</c:v>
+                  <c:v>1910</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>1457</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>853</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>358</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>496</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>1677</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>3440</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>9064</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2</c:v>
+                  <c:v>18880</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5</c:v>
+                  <c:v>37808</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>30</c:v>
+                  <c:v>287194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -795,7 +795,7 @@
         <v>-0.85</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -811,7 +811,7 @@
         <v>-0.75</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -819,7 +819,7 @@
         <v>-0.7</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -827,7 +827,7 @@
         <v>-0.6499999999999999</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>719</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -835,7 +835,7 @@
         <v>-0.6</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>808</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -843,7 +843,7 @@
         <v>-0.55</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -851,7 +851,7 @@
         <v>-0.5</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -859,7 +859,7 @@
         <v>-0.45</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>817</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -867,7 +867,7 @@
         <v>-0.3999999999999999</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>680</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -875,7 +875,7 @@
         <v>-0.35</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -883,7 +883,7 @@
         <v>-0.2999999999999999</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -891,7 +891,7 @@
         <v>-0.25</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>696</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -899,7 +899,7 @@
         <v>-0.2</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -907,7 +907,7 @@
         <v>-0.1499999999999999</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -915,7 +915,7 @@
         <v>-0.09999999999999998</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -923,7 +923,7 @@
         <v>-0.04999999999999993</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>3872</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -939,7 +939,7 @@
         <v>0.05000000000000004</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>5790</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -947,7 +947,7 @@
         <v>0.1000000000000001</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>6045</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -955,7 +955,7 @@
         <v>0.1500000000000001</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>4763</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -963,7 +963,7 @@
         <v>0.2000000000000002</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -971,7 +971,7 @@
         <v>0.25</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -979,7 +979,7 @@
         <v>0.3</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -987,7 +987,7 @@
         <v>0.3500000000000001</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -995,7 +995,7 @@
         <v>0.4000000000000001</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1003,7 +1003,7 @@
         <v>0.4500000000000002</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>853</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1011,7 +1011,7 @@
         <v>0.5</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1019,7 +1019,7 @@
         <v>0.55</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1027,7 +1027,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1035,7 +1035,7 @@
         <v>0.6500000000000001</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1043,7 +1043,7 @@
         <v>0.7000000000000002</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>496</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1051,7 +1051,7 @@
         <v>0.75</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1059,7 +1059,7 @@
         <v>0.8</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1067,7 +1067,7 @@
         <v>0.8500000000000001</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>9064</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1075,7 +1075,7 @@
         <v>0.9000000000000001</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>18880</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1083,7 +1083,7 @@
         <v>0.9500000000000002</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>37808</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1091,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="B41">
-        <v>30</v>
+        <v>287194</v>
       </c>
     </row>
     <row r="42" spans="1:2">

</xml_diff>

<commit_message>
Fixed skipped counting issue
</commit_message>
<xml_diff>
--- a/Pearsons_CC/Python_Code/histogram.sample.xlsx
+++ b/Pearsons_CC/Python_Code/histogram.sample.xlsx
@@ -242,118 +242,118 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>305</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>719</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>808</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>570</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1080</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>817</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>680</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>275</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>353</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>696</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1148</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2042</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2192</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2637</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3872</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5790</c:v>
+                  <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6045</c:v>
+                  <c:v>581</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4763</c:v>
+                  <c:v>519</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3008</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2435</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2280</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1910</c:v>
+                  <c:v>181</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1457</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>853</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>358</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>88</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>79</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>166</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>496</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1677</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3440</c:v>
+                  <c:v>405</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9064</c:v>
+                  <c:v>1005</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>18880</c:v>
+                  <c:v>2075</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>37808</c:v>
+                  <c:v>3963</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>287194</c:v>
+                  <c:v>31328</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -795,7 +795,7 @@
         <v>-0.85</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -811,7 +811,7 @@
         <v>-0.75</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -819,7 +819,7 @@
         <v>-0.7</v>
       </c>
       <c r="B7">
-        <v>305</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -827,7 +827,7 @@
         <v>-0.6499999999999999</v>
       </c>
       <c r="B8">
-        <v>719</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -835,7 +835,7 @@
         <v>-0.6</v>
       </c>
       <c r="B9">
-        <v>808</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -843,7 +843,7 @@
         <v>-0.55</v>
       </c>
       <c r="B10">
-        <v>570</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -851,7 +851,7 @@
         <v>-0.5</v>
       </c>
       <c r="B11">
-        <v>1080</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -859,7 +859,7 @@
         <v>-0.45</v>
       </c>
       <c r="B12">
-        <v>817</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -867,7 +867,7 @@
         <v>-0.3999999999999999</v>
       </c>
       <c r="B13">
-        <v>680</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -875,7 +875,7 @@
         <v>-0.35</v>
       </c>
       <c r="B14">
-        <v>275</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -883,7 +883,7 @@
         <v>-0.2999999999999999</v>
       </c>
       <c r="B15">
-        <v>353</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -891,7 +891,7 @@
         <v>-0.25</v>
       </c>
       <c r="B16">
-        <v>696</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -899,7 +899,7 @@
         <v>-0.2</v>
       </c>
       <c r="B17">
-        <v>1148</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -907,7 +907,7 @@
         <v>-0.1499999999999999</v>
       </c>
       <c r="B18">
-        <v>2042</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -915,7 +915,7 @@
         <v>-0.09999999999999998</v>
       </c>
       <c r="B19">
-        <v>2192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -923,7 +923,7 @@
         <v>-0.04999999999999993</v>
       </c>
       <c r="B20">
-        <v>2637</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <v>3872</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -939,7 +939,7 @@
         <v>0.05000000000000004</v>
       </c>
       <c r="B22">
-        <v>5790</v>
+        <v>555</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -947,7 +947,7 @@
         <v>0.1000000000000001</v>
       </c>
       <c r="B23">
-        <v>6045</v>
+        <v>581</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -955,7 +955,7 @@
         <v>0.1500000000000001</v>
       </c>
       <c r="B24">
-        <v>4763</v>
+        <v>519</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -963,7 +963,7 @@
         <v>0.2000000000000002</v>
       </c>
       <c r="B25">
-        <v>3008</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -971,7 +971,7 @@
         <v>0.25</v>
       </c>
       <c r="B26">
-        <v>2435</v>
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -979,7 +979,7 @@
         <v>0.3</v>
       </c>
       <c r="B27">
-        <v>2280</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -987,7 +987,7 @@
         <v>0.3500000000000001</v>
       </c>
       <c r="B28">
-        <v>1910</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -995,7 +995,7 @@
         <v>0.4000000000000001</v>
       </c>
       <c r="B29">
-        <v>1457</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1003,7 +1003,7 @@
         <v>0.4500000000000002</v>
       </c>
       <c r="B30">
-        <v>853</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1011,7 +1011,7 @@
         <v>0.5</v>
       </c>
       <c r="B31">
-        <v>358</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1019,7 +1019,7 @@
         <v>0.55</v>
       </c>
       <c r="B32">
-        <v>88</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1027,7 +1027,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="B33">
-        <v>79</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1035,7 +1035,7 @@
         <v>0.6500000000000001</v>
       </c>
       <c r="B34">
-        <v>166</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1043,7 +1043,7 @@
         <v>0.7000000000000002</v>
       </c>
       <c r="B35">
-        <v>496</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1051,7 +1051,7 @@
         <v>0.75</v>
       </c>
       <c r="B36">
-        <v>1677</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1059,7 +1059,7 @@
         <v>0.8</v>
       </c>
       <c r="B37">
-        <v>3440</v>
+        <v>405</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1067,7 +1067,7 @@
         <v>0.8500000000000001</v>
       </c>
       <c r="B38">
-        <v>9064</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1075,7 +1075,7 @@
         <v>0.9000000000000001</v>
       </c>
       <c r="B39">
-        <v>18880</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1083,7 +1083,7 @@
         <v>0.9500000000000002</v>
       </c>
       <c r="B40">
-        <v>37808</v>
+        <v>3963</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1091,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="B41">
-        <v>287194</v>
+        <v>31328</v>
       </c>
     </row>
     <row r="42" spans="1:2">

</xml_diff>

<commit_message>
approach 2 try 1
</commit_message>
<xml_diff>
--- a/Pearsons_CC/Python_Code/histogram.sample.xlsx
+++ b/Pearsons_CC/Python_Code/histogram.sample.xlsx
@@ -2280,235 +2280,235 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="322">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="323">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="374">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="324">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="334">
+                <c:pt idx="375">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>503</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>606</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>973</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>994</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>799</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>738</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>663</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="397">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="335">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>114</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>147</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>159</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>176</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>178</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>189</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>194</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>231</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>284</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>273</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>283</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>333</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>328</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>331</c:v>
-                </c:pt>
-                <c:pt idx="365">
-                  <c:v>362</c:v>
-                </c:pt>
-                <c:pt idx="366">
-                  <c:v>326</c:v>
-                </c:pt>
-                <c:pt idx="367">
-                  <c:v>318</c:v>
-                </c:pt>
-                <c:pt idx="368">
-                  <c:v>367</c:v>
-                </c:pt>
-                <c:pt idx="369">
-                  <c:v>358</c:v>
-                </c:pt>
-                <c:pt idx="370">
-                  <c:v>380</c:v>
-                </c:pt>
-                <c:pt idx="371">
-                  <c:v>344</c:v>
-                </c:pt>
-                <c:pt idx="372">
-                  <c:v>401</c:v>
-                </c:pt>
-                <c:pt idx="373">
-                  <c:v>378</c:v>
-                </c:pt>
-                <c:pt idx="374">
-                  <c:v>361</c:v>
-                </c:pt>
-                <c:pt idx="375">
-                  <c:v>321</c:v>
-                </c:pt>
-                <c:pt idx="376">
-                  <c:v>287</c:v>
-                </c:pt>
-                <c:pt idx="377">
-                  <c:v>225</c:v>
-                </c:pt>
-                <c:pt idx="378">
-                  <c:v>171</c:v>
-                </c:pt>
-                <c:pt idx="379">
-                  <c:v>109</c:v>
-                </c:pt>
-                <c:pt idx="380">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="381">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="382">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="383">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="384">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="385">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="386">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="387">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="388">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="389">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="390">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="391">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="392">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="393">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="394">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="395">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="396">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="397">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="398">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="399">
                   <c:v>0</c:v>
@@ -2633,306 +2633,567 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Randomness_Check!$A$1:$A$82</c:f>
+              <c:f>Randomness_Check!$A$1:$A$171</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="82"/>
+                <c:ptCount val="171"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>11</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Randomness_Check!$B$1:$B$82</c:f>
+              <c:f>Randomness_Check!$B$1:$B$171</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="82"/>
+                <c:ptCount val="171"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1689</c:v>
+                  <c:v>730</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1665</c:v>
+                  <c:v>709</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1702</c:v>
+                  <c:v>726</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1713</c:v>
+                  <c:v>696</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1708</c:v>
+                  <c:v>760</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1748</c:v>
+                  <c:v>741</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1745</c:v>
+                  <c:v>677</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1753</c:v>
+                  <c:v>736</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1657</c:v>
+                  <c:v>732</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1754</c:v>
+                  <c:v>724</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1741</c:v>
+                  <c:v>716</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1769</c:v>
+                  <c:v>678</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1774</c:v>
+                  <c:v>695</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1703</c:v>
+                  <c:v>676</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1753</c:v>
+                  <c:v>651</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1694</c:v>
+                  <c:v>736</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1741</c:v>
+                  <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1717</c:v>
+                  <c:v>703</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1703</c:v>
+                  <c:v>682</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1779</c:v>
+                  <c:v>742</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1716</c:v>
+                  <c:v>737</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1763</c:v>
+                  <c:v>683</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1657</c:v>
+                  <c:v>733</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1692</c:v>
+                  <c:v>710</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1716</c:v>
+                  <c:v>671</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1716</c:v>
+                  <c:v>735</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1718</c:v>
+                  <c:v>726</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1729</c:v>
+                  <c:v>734</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1682</c:v>
+                  <c:v>721</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1734</c:v>
+                  <c:v>697</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1688</c:v>
+                  <c:v>696</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1680</c:v>
+                  <c:v>708</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1764</c:v>
+                  <c:v>680</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1696</c:v>
+                  <c:v>744</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1769</c:v>
+                  <c:v>727</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1730</c:v>
+                  <c:v>691</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1791</c:v>
+                  <c:v>762</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1697</c:v>
+                  <c:v>761</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1682</c:v>
+                  <c:v>681</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1758</c:v>
+                  <c:v>712</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1721</c:v>
+                  <c:v>675</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1680</c:v>
+                  <c:v>695</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1771</c:v>
+                  <c:v>644</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1735</c:v>
+                  <c:v>709</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1692</c:v>
+                  <c:v>710</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1740</c:v>
+                  <c:v>696</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1768</c:v>
+                  <c:v>707</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1714</c:v>
+                  <c:v>722</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1722</c:v>
+                  <c:v>703</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1696</c:v>
+                  <c:v>667</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1758</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1754</c:v>
+                  <c:v>702</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1801</c:v>
+                  <c:v>740</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1771</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1735</c:v>
+                  <c:v>671</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1696</c:v>
+                  <c:v>727</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1699</c:v>
+                  <c:v>744</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1772</c:v>
+                  <c:v>717</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1796</c:v>
+                  <c:v>696</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1675</c:v>
+                  <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1661</c:v>
+                  <c:v>675</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1714</c:v>
+                  <c:v>701</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1805</c:v>
+                  <c:v>691</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1701</c:v>
+                  <c:v>716</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1731</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1728</c:v>
+                  <c:v>632</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1713</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1770</c:v>
+                  <c:v>699</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1746</c:v>
+                  <c:v>727</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1720</c:v>
+                  <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1674</c:v>
+                  <c:v>705</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1741</c:v>
+                  <c:v>679</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1712</c:v>
+                  <c:v>701</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1715</c:v>
+                  <c:v>732</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1728</c:v>
+                  <c:v>704</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1721</c:v>
+                  <c:v>677</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1788</c:v>
+                  <c:v>684</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1770</c:v>
+                  <c:v>741</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1777</c:v>
+                  <c:v>766</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1695</c:v>
+                  <c:v>663</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1808</c:v>
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>691</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>693</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>701</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>718</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>668</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>662</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>762</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>693</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>741</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>677</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>674</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>708</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>703</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>688</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>679</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>691</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>667</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>698</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>693</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>753</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>702</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>707</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>731</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>663</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>674</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>701</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>706</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>688</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5961,7 +6222,7 @@
         <v>0.6100000000000001</v>
       </c>
       <c r="B323">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -5969,7 +6230,7 @@
         <v>0.615</v>
       </c>
       <c r="B324">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -5977,7 +6238,7 @@
         <v>0.6200000000000001</v>
       </c>
       <c r="B325">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -5985,7 +6246,7 @@
         <v>0.625</v>
       </c>
       <c r="B326">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -5993,7 +6254,7 @@
         <v>0.6300000000000001</v>
       </c>
       <c r="B327">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -6001,7 +6262,7 @@
         <v>0.635</v>
       </c>
       <c r="B328">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -6009,7 +6270,7 @@
         <v>0.6400000000000001</v>
       </c>
       <c r="B329">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -6017,7 +6278,7 @@
         <v>0.645</v>
       </c>
       <c r="B330">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -6025,7 +6286,7 @@
         <v>0.6500000000000001</v>
       </c>
       <c r="B331">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -6033,7 +6294,7 @@
         <v>0.655</v>
       </c>
       <c r="B332">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -6041,7 +6302,7 @@
         <v>0.6600000000000001</v>
       </c>
       <c r="B333">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -6049,7 +6310,7 @@
         <v>0.665</v>
       </c>
       <c r="B334">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -6057,7 +6318,7 @@
         <v>0.6699999999999999</v>
       </c>
       <c r="B335">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -6065,7 +6326,7 @@
         <v>0.675</v>
       </c>
       <c r="B336">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -6073,7 +6334,7 @@
         <v>0.6799999999999999</v>
       </c>
       <c r="B337">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -6081,7 +6342,7 @@
         <v>0.6850000000000001</v>
       </c>
       <c r="B338">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -6089,7 +6350,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="B339">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -6097,7 +6358,7 @@
         <v>0.6950000000000001</v>
       </c>
       <c r="B340">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -6105,7 +6366,7 @@
         <v>0.7</v>
       </c>
       <c r="B341">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -6113,7 +6374,7 @@
         <v>0.7050000000000001</v>
       </c>
       <c r="B342">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -6121,7 +6382,7 @@
         <v>0.71</v>
       </c>
       <c r="B343">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -6129,7 +6390,7 @@
         <v>0.7150000000000001</v>
       </c>
       <c r="B344">
-        <v>94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -6137,7 +6398,7 @@
         <v>0.72</v>
       </c>
       <c r="B345">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -6145,7 +6406,7 @@
         <v>0.7250000000000001</v>
       </c>
       <c r="B346">
-        <v>119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -6153,7 +6414,7 @@
         <v>0.73</v>
       </c>
       <c r="B347">
-        <v>114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -6161,7 +6422,7 @@
         <v>0.7350000000000001</v>
       </c>
       <c r="B348">
-        <v>121</v>
+        <v>0</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -6169,7 +6430,7 @@
         <v>0.74</v>
       </c>
       <c r="B349">
-        <v>147</v>
+        <v>0</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -6177,7 +6438,7 @@
         <v>0.7450000000000001</v>
       </c>
       <c r="B350">
-        <v>159</v>
+        <v>0</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -6185,7 +6446,7 @@
         <v>0.75</v>
       </c>
       <c r="B351">
-        <v>176</v>
+        <v>0</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -6193,7 +6454,7 @@
         <v>0.7550000000000001</v>
       </c>
       <c r="B352">
-        <v>178</v>
+        <v>0</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -6201,7 +6462,7 @@
         <v>0.76</v>
       </c>
       <c r="B353">
-        <v>189</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -6209,7 +6470,7 @@
         <v>0.7650000000000001</v>
       </c>
       <c r="B354">
-        <v>198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -6217,7 +6478,7 @@
         <v>0.77</v>
       </c>
       <c r="B355">
-        <v>194</v>
+        <v>0</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -6225,7 +6486,7 @@
         <v>0.7750000000000001</v>
       </c>
       <c r="B356">
-        <v>209</v>
+        <v>0</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -6233,7 +6494,7 @@
         <v>0.78</v>
       </c>
       <c r="B357">
-        <v>216</v>
+        <v>0</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -6241,7 +6502,7 @@
         <v>0.7850000000000001</v>
       </c>
       <c r="B358">
-        <v>220</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -6249,7 +6510,7 @@
         <v>0.79</v>
       </c>
       <c r="B359">
-        <v>231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -6257,7 +6518,7 @@
         <v>0.7949999999999999</v>
       </c>
       <c r="B360">
-        <v>284</v>
+        <v>0</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -6265,7 +6526,7 @@
         <v>0.8</v>
       </c>
       <c r="B361">
-        <v>273</v>
+        <v>0</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -6273,7 +6534,7 @@
         <v>0.8049999999999999</v>
       </c>
       <c r="B362">
-        <v>283</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -6281,7 +6542,7 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="B363">
-        <v>333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -6289,7 +6550,7 @@
         <v>0.8149999999999999</v>
       </c>
       <c r="B364">
-        <v>328</v>
+        <v>0</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -6297,7 +6558,7 @@
         <v>0.8200000000000001</v>
       </c>
       <c r="B365">
-        <v>331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -6305,7 +6566,7 @@
         <v>0.825</v>
       </c>
       <c r="B366">
-        <v>362</v>
+        <v>0</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -6313,7 +6574,7 @@
         <v>0.8300000000000001</v>
       </c>
       <c r="B367">
-        <v>326</v>
+        <v>0</v>
       </c>
     </row>
     <row r="368" spans="1:2">
@@ -6321,7 +6582,7 @@
         <v>0.835</v>
       </c>
       <c r="B368">
-        <v>318</v>
+        <v>0</v>
       </c>
     </row>
     <row r="369" spans="1:2">
@@ -6329,7 +6590,7 @@
         <v>0.8400000000000001</v>
       </c>
       <c r="B369">
-        <v>367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="370" spans="1:2">
@@ -6337,7 +6598,7 @@
         <v>0.845</v>
       </c>
       <c r="B370">
-        <v>358</v>
+        <v>0</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -6345,7 +6606,7 @@
         <v>0.8500000000000001</v>
       </c>
       <c r="B371">
-        <v>380</v>
+        <v>0</v>
       </c>
     </row>
     <row r="372" spans="1:2">
@@ -6353,7 +6614,7 @@
         <v>0.855</v>
       </c>
       <c r="B372">
-        <v>344</v>
+        <v>0</v>
       </c>
     </row>
     <row r="373" spans="1:2">
@@ -6361,7 +6622,7 @@
         <v>0.8600000000000001</v>
       </c>
       <c r="B373">
-        <v>401</v>
+        <v>1</v>
       </c>
     </row>
     <row r="374" spans="1:2">
@@ -6369,7 +6630,7 @@
         <v>0.865</v>
       </c>
       <c r="B374">
-        <v>378</v>
+        <v>1</v>
       </c>
     </row>
     <row r="375" spans="1:2">
@@ -6377,7 +6638,7 @@
         <v>0.8700000000000001</v>
       </c>
       <c r="B375">
-        <v>361</v>
+        <v>3</v>
       </c>
     </row>
     <row r="376" spans="1:2">
@@ -6385,7 +6646,7 @@
         <v>0.875</v>
       </c>
       <c r="B376">
-        <v>321</v>
+        <v>10</v>
       </c>
     </row>
     <row r="377" spans="1:2">
@@ -6393,7 +6654,7 @@
         <v>0.8800000000000001</v>
       </c>
       <c r="B377">
-        <v>287</v>
+        <v>16</v>
       </c>
     </row>
     <row r="378" spans="1:2">
@@ -6401,7 +6662,7 @@
         <v>0.885</v>
       </c>
       <c r="B378">
-        <v>225</v>
+        <v>29</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -6409,7 +6670,7 @@
         <v>0.8900000000000001</v>
       </c>
       <c r="B379">
-        <v>171</v>
+        <v>49</v>
       </c>
     </row>
     <row r="380" spans="1:2">
@@ -6417,7 +6678,7 @@
         <v>0.895</v>
       </c>
       <c r="B380">
-        <v>109</v>
+        <v>70</v>
       </c>
     </row>
     <row r="381" spans="1:2">
@@ -6425,7 +6686,7 @@
         <v>0.9000000000000001</v>
       </c>
       <c r="B381">
-        <v>73</v>
+        <v>119</v>
       </c>
     </row>
     <row r="382" spans="1:2">
@@ -6433,7 +6694,7 @@
         <v>0.905</v>
       </c>
       <c r="B382">
-        <v>33</v>
+        <v>180</v>
       </c>
     </row>
     <row r="383" spans="1:2">
@@ -6441,7 +6702,7 @@
         <v>0.9100000000000001</v>
       </c>
       <c r="B383">
-        <v>15</v>
+        <v>257</v>
       </c>
     </row>
     <row r="384" spans="1:2">
@@ -6449,7 +6710,7 @@
         <v>0.915</v>
       </c>
       <c r="B384">
-        <v>7</v>
+        <v>333</v>
       </c>
     </row>
     <row r="385" spans="1:2">
@@ -6457,7 +6718,7 @@
         <v>0.9199999999999999</v>
       </c>
       <c r="B385">
-        <v>2</v>
+        <v>503</v>
       </c>
     </row>
     <row r="386" spans="1:2">
@@ -6465,7 +6726,7 @@
         <v>0.925</v>
       </c>
       <c r="B386">
-        <v>0</v>
+        <v>606</v>
       </c>
     </row>
     <row r="387" spans="1:2">
@@ -6473,7 +6734,7 @@
         <v>0.9299999999999999</v>
       </c>
       <c r="B387">
-        <v>0</v>
+        <v>724</v>
       </c>
     </row>
     <row r="388" spans="1:2">
@@ -6481,7 +6742,7 @@
         <v>0.9350000000000001</v>
       </c>
       <c r="B388">
-        <v>0</v>
+        <v>764</v>
       </c>
     </row>
     <row r="389" spans="1:2">
@@ -6489,7 +6750,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B389">
-        <v>0</v>
+        <v>973</v>
       </c>
     </row>
     <row r="390" spans="1:2">
@@ -6497,7 +6758,7 @@
         <v>0.9450000000000001</v>
       </c>
       <c r="B390">
-        <v>0</v>
+        <v>994</v>
       </c>
     </row>
     <row r="391" spans="1:2">
@@ -6505,7 +6766,7 @@
         <v>0.95</v>
       </c>
       <c r="B391">
-        <v>0</v>
+        <v>830</v>
       </c>
     </row>
     <row r="392" spans="1:2">
@@ -6513,7 +6774,7 @@
         <v>0.9550000000000001</v>
       </c>
       <c r="B392">
-        <v>0</v>
+        <v>799</v>
       </c>
     </row>
     <row r="393" spans="1:2">
@@ -6521,7 +6782,7 @@
         <v>0.96</v>
       </c>
       <c r="B393">
-        <v>0</v>
+        <v>738</v>
       </c>
     </row>
     <row r="394" spans="1:2">
@@ -6529,7 +6790,7 @@
         <v>0.9650000000000001</v>
       </c>
       <c r="B394">
-        <v>0</v>
+        <v>737</v>
       </c>
     </row>
     <row r="395" spans="1:2">
@@ -6537,7 +6798,7 @@
         <v>0.97</v>
       </c>
       <c r="B395">
-        <v>0</v>
+        <v>663</v>
       </c>
     </row>
     <row r="396" spans="1:2">
@@ -6545,7 +6806,7 @@
         <v>0.9750000000000001</v>
       </c>
       <c r="B396">
-        <v>0</v>
+        <v>401</v>
       </c>
     </row>
     <row r="397" spans="1:2">
@@ -6553,7 +6814,7 @@
         <v>0.98</v>
       </c>
       <c r="B397">
-        <v>0</v>
+        <v>167</v>
       </c>
     </row>
     <row r="398" spans="1:2">
@@ -6561,7 +6822,7 @@
         <v>0.9850000000000001</v>
       </c>
       <c r="B398">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="399" spans="1:2">
@@ -6569,7 +6830,7 @@
         <v>0.99</v>
       </c>
       <c r="B399">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400" spans="1:2">
@@ -6605,7 +6866,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B171"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6613,7 +6874,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6621,446 +6882,885 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="B2">
-        <v>1689</v>
+        <v>730</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>1665</v>
+        <v>709</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B4">
-        <v>1702</v>
+        <v>726</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="B5">
-        <v>1713</v>
+        <v>696</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="B6">
-        <v>1708</v>
+        <v>760</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="B7">
-        <v>1748</v>
+        <v>741</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>1745</v>
+        <v>677</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B9">
-        <v>1753</v>
+        <v>736</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>1657</v>
+        <v>732</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="B11">
-        <v>1754</v>
+        <v>724</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B12">
-        <v>1741</v>
+        <v>716</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13">
-        <v>29</v>
-      </c>
       <c r="B13">
-        <v>1769</v>
+        <v>678</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14">
-        <v>11</v>
-      </c>
       <c r="B14">
-        <v>1774</v>
+        <v>695</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15">
-        <v>1703</v>
+        <v>676</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16">
-        <v>1753</v>
+        <v>651</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17">
-        <v>1694</v>
+        <v>736</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18">
-        <v>1741</v>
+        <v>668</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19">
-        <v>1717</v>
+        <v>703</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20">
-        <v>1703</v>
+        <v>682</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21">
-        <v>1779</v>
+        <v>742</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22">
-        <v>1716</v>
+        <v>737</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23">
-        <v>1763</v>
+        <v>683</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24">
-        <v>1657</v>
+        <v>733</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25">
-        <v>1692</v>
+        <v>710</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26">
-        <v>1716</v>
+        <v>671</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27">
-        <v>1716</v>
+        <v>735</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28">
-        <v>1718</v>
+        <v>726</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29">
-        <v>1729</v>
+        <v>734</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30">
-        <v>1682</v>
+        <v>721</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31">
-        <v>1734</v>
+        <v>697</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32">
-        <v>1688</v>
+        <v>696</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33">
-        <v>1680</v>
+        <v>708</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34">
-        <v>1764</v>
+        <v>680</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35">
-        <v>1696</v>
+        <v>744</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36">
-        <v>1769</v>
+        <v>727</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37">
-        <v>1730</v>
+        <v>691</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38">
-        <v>1791</v>
+        <v>762</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39">
-        <v>1697</v>
+        <v>761</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40">
-        <v>1682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41">
-        <v>1758</v>
+        <v>712</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42">
-        <v>1721</v>
+        <v>675</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43">
-        <v>1680</v>
+        <v>695</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44">
-        <v>1771</v>
+        <v>644</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45">
-        <v>1735</v>
+        <v>709</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46">
-        <v>1692</v>
+        <v>710</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47">
-        <v>1740</v>
+        <v>696</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48">
-        <v>1768</v>
+        <v>707</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49">
-        <v>1714</v>
+        <v>722</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50">
-        <v>1722</v>
+        <v>703</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51">
-        <v>1696</v>
+        <v>667</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52">
-        <v>1758</v>
+        <v>660</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53">
-        <v>1754</v>
+        <v>702</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54">
-        <v>1801</v>
+        <v>740</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55">
-        <v>1771</v>
+        <v>670</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56">
-        <v>1735</v>
+        <v>671</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57">
-        <v>1696</v>
+        <v>727</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58">
-        <v>1699</v>
+        <v>744</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59">
-        <v>1772</v>
+        <v>717</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60">
-        <v>1796</v>
+        <v>696</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61">
-        <v>1675</v>
+        <v>668</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62">
-        <v>1661</v>
+        <v>675</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63">
-        <v>1714</v>
+        <v>701</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64">
-        <v>1805</v>
+        <v>691</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65">
-        <v>1701</v>
+        <v>716</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66">
-        <v>1731</v>
+        <v>720</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67">
-        <v>1728</v>
+        <v>632</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68">
-        <v>1713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69">
-        <v>1770</v>
+        <v>699</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70">
-        <v>1746</v>
+        <v>727</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71">
-        <v>1720</v>
+        <v>668</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72">
-        <v>1674</v>
+        <v>705</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73">
-        <v>1741</v>
+        <v>679</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74">
-        <v>1712</v>
+        <v>701</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75">
-        <v>1715</v>
+        <v>732</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76">
-        <v>1728</v>
+        <v>704</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77">
-        <v>1721</v>
+        <v>677</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78">
-        <v>1788</v>
+        <v>684</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79">
-        <v>1770</v>
+        <v>741</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80">
-        <v>1777</v>
+        <v>766</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81">
-        <v>1695</v>
+        <v>663</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82">
-        <v>1808</v>
+        <v>712</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2">
+      <c r="B138">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2">
+      <c r="B139">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2">
+      <c r="B143">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2">
+      <c r="B144">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2">
+      <c r="B146">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2">
+      <c r="B147">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2">
+      <c r="B148">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2">
+      <c r="B149">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2">
+      <c r="B150">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2">
+      <c r="B151">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2">
+      <c r="B152">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2">
+      <c r="B154">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2">
+      <c r="B155">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2">
+      <c r="B156">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2">
+      <c r="B157">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2">
+      <c r="B158">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2">
+      <c r="B159">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2">
+      <c r="B160">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2">
+      <c r="B161">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2">
+      <c r="B162">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2">
+      <c r="B163">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2">
+      <c r="B164">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2">
+      <c r="B165">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2">
+      <c r="B168">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2">
+      <c r="B169">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2">
+      <c r="B170">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171">
+        <v>726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
approach 2 try 2
</commit_message>
<xml_diff>
--- a/Pearsons_CC/Python_Code/histogram.sample.xlsx
+++ b/Pearsons_CC/Python_Code/histogram.sample.xlsx
@@ -2223,7 +2223,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="303">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="304">
                   <c:v>0</c:v>
@@ -2259,256 +2259,256 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="315">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="316">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="317">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="318">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="319">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="320">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="321">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="322">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="323">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="324">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="325">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="326">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="327">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="328">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="329">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="330">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="331">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="332">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="333">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="334">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="335">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="336">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="337">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="338">
-                  <c:v>0</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="339">
-                  <c:v>0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="340">
-                  <c:v>0</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="341">
-                  <c:v>0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="342">
-                  <c:v>0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="343">
-                  <c:v>0</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="344">
-                  <c:v>0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="345">
-                  <c:v>0</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="346">
-                  <c:v>0</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="347">
-                  <c:v>0</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="348">
-                  <c:v>0</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="349">
-                  <c:v>0</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="350">
-                  <c:v>0</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="351">
-                  <c:v>0</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="352">
-                  <c:v>0</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="353">
-                  <c:v>0</c:v>
+                  <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="354">
-                  <c:v>0</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="355">
-                  <c:v>0</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="356">
-                  <c:v>0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="357">
-                  <c:v>0</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="358">
-                  <c:v>0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="359">
-                  <c:v>0</c:v>
+                  <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="360">
-                  <c:v>0</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="361">
-                  <c:v>0</c:v>
+                  <c:v>313</c:v>
                 </c:pt>
                 <c:pt idx="362">
-                  <c:v>0</c:v>
+                  <c:v>339</c:v>
                 </c:pt>
                 <c:pt idx="363">
-                  <c:v>0</c:v>
+                  <c:v>387</c:v>
                 </c:pt>
                 <c:pt idx="364">
-                  <c:v>0</c:v>
+                  <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="365">
-                  <c:v>0</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="366">
-                  <c:v>0</c:v>
+                  <c:v>342</c:v>
                 </c:pt>
                 <c:pt idx="367">
-                  <c:v>0</c:v>
+                  <c:v>355</c:v>
                 </c:pt>
                 <c:pt idx="368">
-                  <c:v>0</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="369">
-                  <c:v>0</c:v>
+                  <c:v>330</c:v>
                 </c:pt>
                 <c:pt idx="370">
-                  <c:v>0</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="371">
-                  <c:v>0</c:v>
+                  <c:v>314</c:v>
                 </c:pt>
                 <c:pt idx="372">
-                  <c:v>1</c:v>
+                  <c:v>318</c:v>
                 </c:pt>
                 <c:pt idx="373">
-                  <c:v>1</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="374">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="385">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="375">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="376">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="377">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="378">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="379">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="380">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="381">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="382">
-                  <c:v>257</c:v>
-                </c:pt>
-                <c:pt idx="383">
-                  <c:v>333</c:v>
-                </c:pt>
-                <c:pt idx="384">
-                  <c:v>503</c:v>
-                </c:pt>
-                <c:pt idx="385">
-                  <c:v>606</c:v>
-                </c:pt>
                 <c:pt idx="386">
-                  <c:v>724</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="387">
-                  <c:v>764</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="388">
-                  <c:v>973</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="389">
-                  <c:v>994</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="390">
-                  <c:v>830</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="391">
-                  <c:v>799</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="392">
-                  <c:v>738</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="393">
-                  <c:v>737</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="394">
-                  <c:v>663</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="395">
-                  <c:v>401</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="396">
-                  <c:v>167</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="397">
-                  <c:v>32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="398">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="399">
                   <c:v>0</c:v>
@@ -2633,567 +2633,387 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Randomness_Check!$A$1:$A$171</c:f>
+              <c:f>Randomness_Check!$A$1:$A$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="171"/>
+                <c:ptCount val="109"/>
                 <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>96</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>28</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>57</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>117</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>84</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Randomness_Check!$B$1:$B$171</c:f>
+              <c:f>Randomness_Check!$B$1:$B$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="171"/>
+                <c:ptCount val="109"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>730</c:v>
+                  <c:v>1299</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>709</c:v>
+                  <c:v>1263</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>726</c:v>
+                  <c:v>1296</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>696</c:v>
+                  <c:v>1313</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>760</c:v>
+                  <c:v>1253</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>741</c:v>
+                  <c:v>1273</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>677</c:v>
+                  <c:v>1312</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>736</c:v>
+                  <c:v>1296</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>732</c:v>
+                  <c:v>1309</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>724</c:v>
+                  <c:v>1333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>716</c:v>
+                  <c:v>1262</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>678</c:v>
+                  <c:v>1329</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>695</c:v>
+                  <c:v>1364</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>676</c:v>
+                  <c:v>1338</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>651</c:v>
+                  <c:v>1302</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>736</c:v>
+                  <c:v>1271</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>668</c:v>
+                  <c:v>1277</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>703</c:v>
+                  <c:v>1277</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>682</c:v>
+                  <c:v>1314</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>742</c:v>
+                  <c:v>1292</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>737</c:v>
+                  <c:v>1251</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>683</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>733</c:v>
+                  <c:v>1261</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>710</c:v>
+                  <c:v>1289</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>671</c:v>
+                  <c:v>1305</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>735</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>726</c:v>
+                  <c:v>1289</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>734</c:v>
+                  <c:v>1295</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>721</c:v>
+                  <c:v>1306</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>697</c:v>
+                  <c:v>1294</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>696</c:v>
+                  <c:v>1319</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>708</c:v>
+                  <c:v>1306</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>680</c:v>
+                  <c:v>1308</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>744</c:v>
+                  <c:v>1367</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>727</c:v>
+                  <c:v>1287</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>691</c:v>
+                  <c:v>1264</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>762</c:v>
+                  <c:v>1345</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>761</c:v>
+                  <c:v>1284</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>681</c:v>
+                  <c:v>1246</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>712</c:v>
+                  <c:v>1273</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>675</c:v>
+                  <c:v>1334</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>695</c:v>
+                  <c:v>1297</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>644</c:v>
+                  <c:v>1292</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>709</c:v>
+                  <c:v>1278</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>710</c:v>
+                  <c:v>1272</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>696</c:v>
+                  <c:v>1302</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>707</c:v>
+                  <c:v>1262</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>722</c:v>
+                  <c:v>1297</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>703</c:v>
+                  <c:v>1267</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>667</c:v>
+                  <c:v>1336</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>660</c:v>
+                  <c:v>1296</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>702</c:v>
+                  <c:v>1326</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>740</c:v>
+                  <c:v>1321</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>670</c:v>
+                  <c:v>1286</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>671</c:v>
+                  <c:v>1299</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>727</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>744</c:v>
+                  <c:v>1338</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>717</c:v>
+                  <c:v>1322</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>696</c:v>
+                  <c:v>1229</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>668</c:v>
+                  <c:v>1266</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>675</c:v>
+                  <c:v>1324</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>701</c:v>
+                  <c:v>1257</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>691</c:v>
+                  <c:v>1318</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>716</c:v>
+                  <c:v>1310</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>720</c:v>
+                  <c:v>1304</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>632</c:v>
+                  <c:v>1291</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>711</c:v>
+                  <c:v>1241</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>699</c:v>
+                  <c:v>1348</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>727</c:v>
+                  <c:v>1320</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>668</c:v>
+                  <c:v>1291</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>705</c:v>
+                  <c:v>1286</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>679</c:v>
+                  <c:v>1305</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>701</c:v>
+                  <c:v>1277</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>732</c:v>
+                  <c:v>1311</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>704</c:v>
+                  <c:v>1284</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>677</c:v>
+                  <c:v>1318</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>684</c:v>
+                  <c:v>1364</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>741</c:v>
+                  <c:v>1298</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>766</c:v>
+                  <c:v>1338</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>663</c:v>
+                  <c:v>1297</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>712</c:v>
+                  <c:v>1298</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>691</c:v>
+                  <c:v>1298</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>725</c:v>
+                  <c:v>1243</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>704</c:v>
+                  <c:v>1270</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>680</c:v>
+                  <c:v>1278</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>687</c:v>
+                  <c:v>1297</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>676</c:v>
+                  <c:v>1230</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>700</c:v>
+                  <c:v>1336</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>717</c:v>
+                  <c:v>1271</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>711</c:v>
+                  <c:v>1326</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>713</c:v>
+                  <c:v>1276</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>693</c:v>
+                  <c:v>1305</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>721</c:v>
+                  <c:v>1258</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>735</c:v>
+                  <c:v>1395</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>701</c:v>
+                  <c:v>1270</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>723</c:v>
+                  <c:v>1281</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>735</c:v>
+                  <c:v>1251</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>718</c:v>
+                  <c:v>1297</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>684</c:v>
+                  <c:v>1280</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>668</c:v>
+                  <c:v>1346</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>675</c:v>
+                  <c:v>1273</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>662</c:v>
+                  <c:v>1292</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>714</c:v>
+                  <c:v>1305</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>696</c:v>
+                  <c:v>1318</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>720</c:v>
+                  <c:v>1248</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>713</c:v>
+                  <c:v>1308</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>722</c:v>
+                  <c:v>1341</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>660</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>762</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>727</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>693</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>741</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>719</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>737</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>689</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>731</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>742</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>745</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>677</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>705</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>699</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>674</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>728</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>708</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>703</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>688</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>679</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>691</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>724</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>727</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>716</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>667</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>717</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>686</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>746</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>684</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>748</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>698</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>726</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>661</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>739</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>693</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>729</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>715</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>731</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>710</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>753</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>702</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>707</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>699</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>727</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>715</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>728</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>714</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>689</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>696</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>731</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>722</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>663</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>674</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>701</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>706</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>725</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>686</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>687</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>687</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>704</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>688</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>726</c:v>
+                  <c:v>1295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6070,7 +5890,7 @@
         <v>0.5150000000000001</v>
       </c>
       <c r="B304">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -6166,7 +5986,7 @@
         <v>0.575</v>
       </c>
       <c r="B316">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -6182,7 +6002,7 @@
         <v>0.585</v>
       </c>
       <c r="B318">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -6190,7 +6010,7 @@
         <v>0.5900000000000001</v>
       </c>
       <c r="B319">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -6206,7 +6026,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="B321">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -6214,7 +6034,7 @@
         <v>0.605</v>
       </c>
       <c r="B322">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -6222,7 +6042,7 @@
         <v>0.6100000000000001</v>
       </c>
       <c r="B323">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -6230,7 +6050,7 @@
         <v>0.615</v>
       </c>
       <c r="B324">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -6238,7 +6058,7 @@
         <v>0.6200000000000001</v>
       </c>
       <c r="B325">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -6246,7 +6066,7 @@
         <v>0.625</v>
       </c>
       <c r="B326">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -6254,7 +6074,7 @@
         <v>0.6300000000000001</v>
       </c>
       <c r="B327">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -6262,7 +6082,7 @@
         <v>0.635</v>
       </c>
       <c r="B328">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -6270,7 +6090,7 @@
         <v>0.6400000000000001</v>
       </c>
       <c r="B329">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -6278,7 +6098,7 @@
         <v>0.645</v>
       </c>
       <c r="B330">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -6286,7 +6106,7 @@
         <v>0.6500000000000001</v>
       </c>
       <c r="B331">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -6294,7 +6114,7 @@
         <v>0.655</v>
       </c>
       <c r="B332">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -6302,7 +6122,7 @@
         <v>0.6600000000000001</v>
       </c>
       <c r="B333">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -6310,7 +6130,7 @@
         <v>0.665</v>
       </c>
       <c r="B334">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -6318,7 +6138,7 @@
         <v>0.6699999999999999</v>
       </c>
       <c r="B335">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -6326,7 +6146,7 @@
         <v>0.675</v>
       </c>
       <c r="B336">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -6334,7 +6154,7 @@
         <v>0.6799999999999999</v>
       </c>
       <c r="B337">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -6342,7 +6162,7 @@
         <v>0.6850000000000001</v>
       </c>
       <c r="B338">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -6350,7 +6170,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="B339">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -6358,7 +6178,7 @@
         <v>0.6950000000000001</v>
       </c>
       <c r="B340">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -6366,7 +6186,7 @@
         <v>0.7</v>
       </c>
       <c r="B341">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -6374,7 +6194,7 @@
         <v>0.7050000000000001</v>
       </c>
       <c r="B342">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -6382,7 +6202,7 @@
         <v>0.71</v>
       </c>
       <c r="B343">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -6390,7 +6210,7 @@
         <v>0.7150000000000001</v>
       </c>
       <c r="B344">
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -6398,7 +6218,7 @@
         <v>0.72</v>
       </c>
       <c r="B345">
-        <v>0</v>
+        <v>112</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -6406,7 +6226,7 @@
         <v>0.7250000000000001</v>
       </c>
       <c r="B346">
-        <v>0</v>
+        <v>148</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -6414,7 +6234,7 @@
         <v>0.73</v>
       </c>
       <c r="B347">
-        <v>0</v>
+        <v>141</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -6422,7 +6242,7 @@
         <v>0.7350000000000001</v>
       </c>
       <c r="B348">
-        <v>0</v>
+        <v>136</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -6430,7 +6250,7 @@
         <v>0.74</v>
       </c>
       <c r="B349">
-        <v>0</v>
+        <v>169</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -6438,7 +6258,7 @@
         <v>0.7450000000000001</v>
       </c>
       <c r="B350">
-        <v>0</v>
+        <v>198</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -6446,7 +6266,7 @@
         <v>0.75</v>
       </c>
       <c r="B351">
-        <v>0</v>
+        <v>190</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -6454,7 +6274,7 @@
         <v>0.7550000000000001</v>
       </c>
       <c r="B352">
-        <v>0</v>
+        <v>196</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -6462,7 +6282,7 @@
         <v>0.76</v>
       </c>
       <c r="B353">
-        <v>0</v>
+        <v>237</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -6470,7 +6290,7 @@
         <v>0.7650000000000001</v>
       </c>
       <c r="B354">
-        <v>0</v>
+        <v>251</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -6478,7 +6298,7 @@
         <v>0.77</v>
       </c>
       <c r="B355">
-        <v>0</v>
+        <v>278</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -6486,7 +6306,7 @@
         <v>0.7750000000000001</v>
       </c>
       <c r="B356">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -6494,7 +6314,7 @@
         <v>0.78</v>
       </c>
       <c r="B357">
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -6502,7 +6322,7 @@
         <v>0.7850000000000001</v>
       </c>
       <c r="B358">
-        <v>0</v>
+        <v>288</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -6510,7 +6330,7 @@
         <v>0.79</v>
       </c>
       <c r="B359">
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -6518,7 +6338,7 @@
         <v>0.7949999999999999</v>
       </c>
       <c r="B360">
-        <v>0</v>
+        <v>340</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -6526,7 +6346,7 @@
         <v>0.8</v>
       </c>
       <c r="B361">
-        <v>0</v>
+        <v>344</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -6534,7 +6354,7 @@
         <v>0.8049999999999999</v>
       </c>
       <c r="B362">
-        <v>0</v>
+        <v>313</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -6542,7 +6362,7 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="B363">
-        <v>0</v>
+        <v>339</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -6550,7 +6370,7 @@
         <v>0.8149999999999999</v>
       </c>
       <c r="B364">
-        <v>0</v>
+        <v>387</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -6558,7 +6378,7 @@
         <v>0.8200000000000001</v>
       </c>
       <c r="B365">
-        <v>0</v>
+        <v>334</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -6566,7 +6386,7 @@
         <v>0.825</v>
       </c>
       <c r="B366">
-        <v>0</v>
+        <v>360</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -6574,7 +6394,7 @@
         <v>0.8300000000000001</v>
       </c>
       <c r="B367">
-        <v>0</v>
+        <v>342</v>
       </c>
     </row>
     <row r="368" spans="1:2">
@@ -6582,7 +6402,7 @@
         <v>0.835</v>
       </c>
       <c r="B368">
-        <v>0</v>
+        <v>355</v>
       </c>
     </row>
     <row r="369" spans="1:2">
@@ -6590,7 +6410,7 @@
         <v>0.8400000000000001</v>
       </c>
       <c r="B369">
-        <v>0</v>
+        <v>323</v>
       </c>
     </row>
     <row r="370" spans="1:2">
@@ -6598,7 +6418,7 @@
         <v>0.845</v>
       </c>
       <c r="B370">
-        <v>0</v>
+        <v>330</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -6606,7 +6426,7 @@
         <v>0.8500000000000001</v>
       </c>
       <c r="B371">
-        <v>0</v>
+        <v>287</v>
       </c>
     </row>
     <row r="372" spans="1:2">
@@ -6614,7 +6434,7 @@
         <v>0.855</v>
       </c>
       <c r="B372">
-        <v>0</v>
+        <v>314</v>
       </c>
     </row>
     <row r="373" spans="1:2">
@@ -6622,7 +6442,7 @@
         <v>0.8600000000000001</v>
       </c>
       <c r="B373">
-        <v>1</v>
+        <v>318</v>
       </c>
     </row>
     <row r="374" spans="1:2">
@@ -6630,7 +6450,7 @@
         <v>0.865</v>
       </c>
       <c r="B374">
-        <v>1</v>
+        <v>264</v>
       </c>
     </row>
     <row r="375" spans="1:2">
@@ -6638,7 +6458,7 @@
         <v>0.8700000000000001</v>
       </c>
       <c r="B375">
-        <v>3</v>
+        <v>226</v>
       </c>
     </row>
     <row r="376" spans="1:2">
@@ -6646,7 +6466,7 @@
         <v>0.875</v>
       </c>
       <c r="B376">
-        <v>10</v>
+        <v>222</v>
       </c>
     </row>
     <row r="377" spans="1:2">
@@ -6654,7 +6474,7 @@
         <v>0.8800000000000001</v>
       </c>
       <c r="B377">
-        <v>16</v>
+        <v>187</v>
       </c>
     </row>
     <row r="378" spans="1:2">
@@ -6662,7 +6482,7 @@
         <v>0.885</v>
       </c>
       <c r="B378">
-        <v>29</v>
+        <v>157</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -6670,7 +6490,7 @@
         <v>0.8900000000000001</v>
       </c>
       <c r="B379">
-        <v>49</v>
+        <v>127</v>
       </c>
     </row>
     <row r="380" spans="1:2">
@@ -6678,7 +6498,7 @@
         <v>0.895</v>
       </c>
       <c r="B380">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="381" spans="1:2">
@@ -6686,7 +6506,7 @@
         <v>0.9000000000000001</v>
       </c>
       <c r="B381">
-        <v>119</v>
+        <v>50</v>
       </c>
     </row>
     <row r="382" spans="1:2">
@@ -6694,7 +6514,7 @@
         <v>0.905</v>
       </c>
       <c r="B382">
-        <v>180</v>
+        <v>49</v>
       </c>
     </row>
     <row r="383" spans="1:2">
@@ -6702,7 +6522,7 @@
         <v>0.9100000000000001</v>
       </c>
       <c r="B383">
-        <v>257</v>
+        <v>21</v>
       </c>
     </row>
     <row r="384" spans="1:2">
@@ -6710,7 +6530,7 @@
         <v>0.915</v>
       </c>
       <c r="B384">
-        <v>333</v>
+        <v>12</v>
       </c>
     </row>
     <row r="385" spans="1:2">
@@ -6718,7 +6538,7 @@
         <v>0.9199999999999999</v>
       </c>
       <c r="B385">
-        <v>503</v>
+        <v>14</v>
       </c>
     </row>
     <row r="386" spans="1:2">
@@ -6726,7 +6546,7 @@
         <v>0.925</v>
       </c>
       <c r="B386">
-        <v>606</v>
+        <v>3</v>
       </c>
     </row>
     <row r="387" spans="1:2">
@@ -6734,7 +6554,7 @@
         <v>0.9299999999999999</v>
       </c>
       <c r="B387">
-        <v>724</v>
+        <v>3</v>
       </c>
     </row>
     <row r="388" spans="1:2">
@@ -6742,7 +6562,7 @@
         <v>0.9350000000000001</v>
       </c>
       <c r="B388">
-        <v>764</v>
+        <v>0</v>
       </c>
     </row>
     <row r="389" spans="1:2">
@@ -6750,7 +6570,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B389">
-        <v>973</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390" spans="1:2">
@@ -6758,7 +6578,7 @@
         <v>0.9450000000000001</v>
       </c>
       <c r="B390">
-        <v>994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391" spans="1:2">
@@ -6766,7 +6586,7 @@
         <v>0.95</v>
       </c>
       <c r="B391">
-        <v>830</v>
+        <v>0</v>
       </c>
     </row>
     <row r="392" spans="1:2">
@@ -6774,7 +6594,7 @@
         <v>0.9550000000000001</v>
       </c>
       <c r="B392">
-        <v>799</v>
+        <v>0</v>
       </c>
     </row>
     <row r="393" spans="1:2">
@@ -6782,7 +6602,7 @@
         <v>0.96</v>
       </c>
       <c r="B393">
-        <v>738</v>
+        <v>0</v>
       </c>
     </row>
     <row r="394" spans="1:2">
@@ -6790,7 +6610,7 @@
         <v>0.9650000000000001</v>
       </c>
       <c r="B394">
-        <v>737</v>
+        <v>0</v>
       </c>
     </row>
     <row r="395" spans="1:2">
@@ -6798,7 +6618,7 @@
         <v>0.97</v>
       </c>
       <c r="B395">
-        <v>663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="396" spans="1:2">
@@ -6806,7 +6626,7 @@
         <v>0.9750000000000001</v>
       </c>
       <c r="B396">
-        <v>401</v>
+        <v>0</v>
       </c>
     </row>
     <row r="397" spans="1:2">
@@ -6814,7 +6634,7 @@
         <v>0.98</v>
       </c>
       <c r="B397">
-        <v>167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="398" spans="1:2">
@@ -6822,7 +6642,7 @@
         <v>0.9850000000000001</v>
       </c>
       <c r="B398">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="399" spans="1:2">
@@ -6830,7 +6650,7 @@
         <v>0.99</v>
       </c>
       <c r="B399">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="400" spans="1:2">
@@ -6866,7 +6686,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B171"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6874,7 +6694,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6882,885 +6702,581 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>730</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="B3">
-        <v>709</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B4">
-        <v>726</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>117</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>696</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>760</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B7">
-        <v>741</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="B8">
-        <v>677</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>736</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B10">
-        <v>732</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>724</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B12">
-        <v>716</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="13" spans="1:2">
+      <c r="A13">
+        <v>33</v>
+      </c>
       <c r="B13">
-        <v>678</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="14" spans="1:2">
+      <c r="A14">
+        <v>87</v>
+      </c>
       <c r="B14">
-        <v>695</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15">
-        <v>676</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16">
-        <v>651</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17">
-        <v>736</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18">
-        <v>668</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19">
-        <v>703</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20">
-        <v>682</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21">
-        <v>742</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22">
-        <v>737</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23">
-        <v>683</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24">
-        <v>733</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25">
-        <v>710</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26">
-        <v>671</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27">
-        <v>735</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28">
-        <v>726</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29">
-        <v>734</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30">
-        <v>721</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31">
-        <v>697</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32">
-        <v>696</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33">
-        <v>708</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34">
-        <v>680</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35">
-        <v>744</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36">
-        <v>727</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37">
-        <v>691</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38">
-        <v>762</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39">
-        <v>761</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40">
-        <v>681</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41">
-        <v>712</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42">
-        <v>675</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43">
-        <v>695</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44">
-        <v>644</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45">
-        <v>709</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46">
-        <v>710</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47">
-        <v>696</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48">
-        <v>707</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49">
-        <v>722</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50">
-        <v>703</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51">
-        <v>667</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52">
-        <v>660</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53">
-        <v>702</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54">
-        <v>740</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="55" spans="2:2">
       <c r="B55">
-        <v>670</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56">
-        <v>671</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57">
-        <v>727</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58">
-        <v>744</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="59" spans="2:2">
       <c r="B59">
-        <v>717</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60">
-        <v>696</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61">
-        <v>668</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62">
-        <v>675</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63">
-        <v>701</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="64" spans="2:2">
       <c r="B64">
-        <v>691</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65">
-        <v>716</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66">
-        <v>720</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67">
-        <v>632</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68">
-        <v>711</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69">
-        <v>699</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="70" spans="2:2">
       <c r="B70">
-        <v>727</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="71" spans="2:2">
       <c r="B71">
-        <v>668</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="72" spans="2:2">
       <c r="B72">
-        <v>705</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73">
-        <v>679</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74">
-        <v>701</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="75" spans="2:2">
       <c r="B75">
-        <v>732</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="76" spans="2:2">
       <c r="B76">
-        <v>704</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="77" spans="2:2">
       <c r="B77">
-        <v>677</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="78" spans="2:2">
       <c r="B78">
-        <v>684</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="79" spans="2:2">
       <c r="B79">
-        <v>741</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80">
-        <v>766</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81">
-        <v>663</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82">
-        <v>712</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83">
-        <v>691</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="84" spans="2:2">
       <c r="B84">
-        <v>725</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="85" spans="2:2">
       <c r="B85">
-        <v>704</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86">
-        <v>680</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87">
-        <v>687</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88">
-        <v>676</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="89" spans="2:2">
       <c r="B89">
-        <v>700</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="90" spans="2:2">
       <c r="B90">
-        <v>717</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91">
-        <v>711</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="92" spans="2:2">
       <c r="B92">
-        <v>713</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="93" spans="2:2">
       <c r="B93">
-        <v>693</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="94" spans="2:2">
       <c r="B94">
-        <v>721</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="95" spans="2:2">
       <c r="B95">
-        <v>735</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="96" spans="2:2">
       <c r="B96">
-        <v>701</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97">
-        <v>723</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98">
-        <v>735</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99">
-        <v>718</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100">
-        <v>684</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101">
-        <v>668</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102">
-        <v>675</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103">
-        <v>662</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="104" spans="2:2">
       <c r="B104">
-        <v>714</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="105" spans="2:2">
       <c r="B105">
-        <v>696</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="106" spans="2:2">
       <c r="B106">
-        <v>720</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="107" spans="2:2">
       <c r="B107">
-        <v>713</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="108" spans="2:2">
       <c r="B108">
-        <v>722</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="109" spans="2:2">
       <c r="B109">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2">
-      <c r="B110">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="111" spans="2:2">
-      <c r="B111">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="112" spans="2:2">
-      <c r="B112">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2">
-      <c r="B113">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2">
-      <c r="B114">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2">
-      <c r="B115">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2">
-      <c r="B116">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2">
-      <c r="B117">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="118" spans="2:2">
-      <c r="B118">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2">
-      <c r="B119">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="120" spans="2:2">
-      <c r="B120">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2">
-      <c r="B121">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2">
-      <c r="B122">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="123" spans="2:2">
-      <c r="B123">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="124" spans="2:2">
-      <c r="B124">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="125" spans="2:2">
-      <c r="B125">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2">
-      <c r="B126">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="127" spans="2:2">
-      <c r="B127">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="128" spans="2:2">
-      <c r="B128">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="129" spans="2:2">
-      <c r="B129">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="130" spans="2:2">
-      <c r="B130">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2">
-      <c r="B131">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2">
-      <c r="B132">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2">
-      <c r="B133">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2">
-      <c r="B134">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2">
-      <c r="B135">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2">
-      <c r="B136">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2">
-      <c r="B137">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="138" spans="2:2">
-      <c r="B138">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="139" spans="2:2">
-      <c r="B139">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2">
-      <c r="B140">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2">
-      <c r="B141">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2">
-      <c r="B142">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2">
-      <c r="B143">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="144" spans="2:2">
-      <c r="B144">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="145" spans="2:2">
-      <c r="B145">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2">
-      <c r="B146">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="147" spans="2:2">
-      <c r="B147">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="148" spans="2:2">
-      <c r="B148">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2">
-      <c r="B149">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="150" spans="2:2">
-      <c r="B150">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="151" spans="2:2">
-      <c r="B151">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="152" spans="2:2">
-      <c r="B152">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="153" spans="2:2">
-      <c r="B153">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="154" spans="2:2">
-      <c r="B154">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2">
-      <c r="B155">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="156" spans="2:2">
-      <c r="B156">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="157" spans="2:2">
-      <c r="B157">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="158" spans="2:2">
-      <c r="B158">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="159" spans="2:2">
-      <c r="B159">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="160" spans="2:2">
-      <c r="B160">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="161" spans="2:2">
-      <c r="B161">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="162" spans="2:2">
-      <c r="B162">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="163" spans="2:2">
-      <c r="B163">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="164" spans="2:2">
-      <c r="B164">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="165" spans="2:2">
-      <c r="B165">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="166" spans="2:2">
-      <c r="B166">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="167" spans="2:2">
-      <c r="B167">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="168" spans="2:2">
-      <c r="B168">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="169" spans="2:2">
-      <c r="B169">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="170" spans="2:2">
-      <c r="B170">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="171" spans="2:2">
-      <c r="B171">
-        <v>726</v>
+        <v>1295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>